<commit_message>
Folder with excel and pdf files
</commit_message>
<xml_diff>
--- a/output/agencies.xlsx
+++ b/output/agencies.xlsx
@@ -7,168 +7,243 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Agencies" sheetId="1" r:id="rId1"/>
+    <sheet name="Individual Investments" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+  <si>
+    <t>$2.7B</t>
+  </si>
+  <si>
+    <t>$2.8B</t>
+  </si>
+  <si>
+    <t>$36B</t>
+  </si>
+  <si>
+    <t>$7.0B</t>
+  </si>
+  <si>
+    <t>$1.5B</t>
+  </si>
+  <si>
+    <t>$3.1B</t>
+  </si>
+  <si>
+    <t>$819M</t>
+  </si>
+  <si>
+    <t>$2.6B</t>
+  </si>
+  <si>
+    <t>$5.4B</t>
+  </si>
+  <si>
+    <t>$2.0B</t>
+  </si>
+  <si>
+    <t>$1.0B</t>
+  </si>
+  <si>
+    <t>$385M</t>
+  </si>
+  <si>
+    <t>$3.5B</t>
+  </si>
+  <si>
+    <t>$765M</t>
+  </si>
+  <si>
+    <t>$7.4B</t>
+  </si>
+  <si>
+    <t>$447M</t>
+  </si>
+  <si>
+    <t>$2.2B</t>
+  </si>
+  <si>
+    <t>$125M</t>
+  </si>
+  <si>
+    <t>$129M</t>
+  </si>
+  <si>
+    <t>$9.1B</t>
+  </si>
+  <si>
+    <t>$256M</t>
+  </si>
+  <si>
+    <t>$275M</t>
+  </si>
+  <si>
+    <t>$99.9M</t>
+  </si>
+  <si>
+    <t>$136M</t>
+  </si>
+  <si>
+    <t>$141M</t>
+  </si>
   <si>
     <t>Department of Agriculture</t>
   </si>
   <si>
-    <t>$2.7B</t>
-  </si>
-  <si>
     <t>Department of Commerce</t>
   </si>
   <si>
-    <t>$2.8B</t>
-  </si>
-  <si>
     <t>Department of Defense</t>
   </si>
   <si>
-    <t>$36B</t>
-  </si>
-  <si>
     <t>Department of Health and Human Services</t>
   </si>
   <si>
-    <t>$7.0B</t>
-  </si>
-  <si>
     <t>Department of the Interior</t>
   </si>
   <si>
-    <t>$1.5B</t>
-  </si>
-  <si>
     <t>Department of Justice</t>
   </si>
   <si>
-    <t>$3.1B</t>
-  </si>
-  <si>
     <t>Department of Labor</t>
   </si>
   <si>
-    <t>$819M</t>
-  </si>
-  <si>
     <t>Department of State</t>
   </si>
   <si>
-    <t>$2.6B</t>
-  </si>
-  <si>
     <t>Department of the Treasury</t>
   </si>
   <si>
-    <t>$5.4B</t>
-  </si>
-  <si>
     <t>Social Security Administration</t>
   </si>
   <si>
-    <t>$2.0B</t>
-  </si>
-  <si>
     <t>Department of Education</t>
   </si>
   <si>
-    <t>$1.0B</t>
-  </si>
-  <si>
     <t>Department of Energy</t>
   </si>
   <si>
     <t>Environmental Protection Agency</t>
   </si>
   <si>
-    <t>$385M</t>
-  </si>
-  <si>
     <t>Department of Transportation</t>
   </si>
   <si>
-    <t>$3.5B</t>
-  </si>
-  <si>
     <t>General Services Administration</t>
   </si>
   <si>
-    <t>$765M</t>
-  </si>
-  <si>
     <t>Department of Homeland Security</t>
   </si>
   <si>
-    <t>$7.4B</t>
-  </si>
-  <si>
     <t>Department of Housing and Urban Development</t>
   </si>
   <si>
-    <t>$447M</t>
-  </si>
-  <si>
     <t>National Aeronautics and Space Administration</t>
   </si>
   <si>
-    <t>$2.2B</t>
-  </si>
-  <si>
     <t>Office of Personnel Management</t>
   </si>
   <si>
-    <t>$125M</t>
-  </si>
-  <si>
     <t>Small Business Administration</t>
   </si>
   <si>
-    <t>$129M</t>
-  </si>
-  <si>
     <t>Department of Veterans Affairs</t>
   </si>
   <si>
-    <t>$9.1B</t>
-  </si>
-  <si>
     <t>U.S. Agency for International Development</t>
   </si>
   <si>
-    <t>$256M</t>
-  </si>
-  <si>
     <t>U.S. Army Corps of Engineers</t>
   </si>
   <si>
-    <t>$275M</t>
-  </si>
-  <si>
     <t>National Archives and Records Administration</t>
   </si>
   <si>
-    <t>$99.9M</t>
-  </si>
-  <si>
     <t>National Science Foundation</t>
   </si>
   <si>
-    <t>$136M</t>
+    <t>Nuclear Regulatory Commission</t>
+  </si>
+  <si>
+    <t>$5.949</t>
+  </si>
+  <si>
+    <t>$4.416</t>
+  </si>
+  <si>
+    <t>$0.000</t>
+  </si>
+  <si>
+    <t>$2.673</t>
+  </si>
+  <si>
+    <t>$38.700</t>
+  </si>
+  <si>
+    <t>$16.468</t>
+  </si>
+  <si>
+    <t>$26.475</t>
+  </si>
+  <si>
+    <t>$8.369</t>
+  </si>
+  <si>
+    <t>$0.321</t>
+  </si>
+  <si>
+    <t>$33.380</t>
+  </si>
+  <si>
+    <t>005-000000042</t>
+  </si>
+  <si>
+    <t>005-000001838</t>
+  </si>
+  <si>
+    <t>005-000003326</t>
+  </si>
+  <si>
+    <t>005-000003245</t>
+  </si>
+  <si>
+    <t>005-000003440</t>
+  </si>
+  <si>
+    <t>005-000000063</t>
+  </si>
+  <si>
+    <t>005-000003311</t>
+  </si>
+  <si>
+    <t>005-000001870</t>
+  </si>
+  <si>
+    <t>005-000003255</t>
+  </si>
+  <si>
+    <t>005-000003010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -184,7 +259,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -192,12 +267,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,210 +585,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="B1" s="1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>47</v>
       </c>
       <c r="B25" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>